<commit_message>
New Version of Calendar
- New .xlsx of the calendar, the game is now aiming for Content Complete on JULY 26th, to LAUNCH on July 28th
</commit_message>
<xml_diff>
--- a/Handgun Hoedown - Milestones & Waterfall.xlsx
+++ b/Handgun Hoedown - Milestones & Waterfall.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
   <si>
     <t>Week 1</t>
   </si>
@@ -80,12 +80,6 @@
     <t>June 26 - July 1</t>
   </si>
   <si>
-    <t>Create Branch for Mechanics Exploration</t>
-  </si>
-  <si>
-    <t>Playtest Version</t>
-  </si>
-  <si>
     <t>MECHANIC DESIGN
 LOCK</t>
   </si>
@@ -105,31 +99,22 @@
     <t>Sound Design Exploration</t>
   </si>
   <si>
-    <t>Find Background Music Track(s)</t>
-  </si>
-  <si>
     <t>Week 3</t>
   </si>
   <si>
     <t>July 3 - 8</t>
   </si>
   <si>
-    <t>PLAYTEST</t>
+    <t>Wtf are we doing about animations</t>
   </si>
   <si>
-    <t>Character finished + #Screenshot Saturday</t>
+    <t>Chris Blew Up His Hand</t>
   </si>
   <si>
-    <t>New Mechanics Coding</t>
+    <t>Kenny on Vacation</t>
   </si>
   <si>
-    <t>Level Design + Menu Design</t>
-  </si>
-  <si>
-    <t>Process Sound Design</t>
-  </si>
-  <si>
-    <t>Implement Sound Design</t>
+    <t>Finish Music, Further Sound Design</t>
   </si>
   <si>
     <t>Week 4</t>
@@ -138,38 +123,19 @@
     <t>July 10 - 15</t>
   </si>
   <si>
-    <t>CONTENT
-COMPLETE + PLAYTEST</t>
+    <t>PLAYTEST</t>
   </si>
   <si>
-    <t>LOCK BUILD</t>
+    <t>#Screenshot Saturday + PLAYTEST</t>
   </si>
   <si>
-    <t>#Screenshot Saturday</t>
+    <t>Updating Old Code</t>
   </si>
   <si>
-    <t>Come to Blossom St. on TR, F</t>
+    <t>Level Design</t>
   </si>
   <si>
-    <t>Polish Code / QoL Fixes</t>
-  </si>
-  <si>
-    <t>Bugfix</t>
-  </si>
-  <si>
-    <t>QoL = scene transitions, defaults, etc.</t>
-  </si>
-  <si>
-    <t>Implement UI</t>
-  </si>
-  <si>
-    <t>Polish Art Assets / UI</t>
-  </si>
-  <si>
-    <t>Post-Processing / Color Pass</t>
-  </si>
-  <si>
-    <t>Marketing Materials / Page Design</t>
+    <t>Implement Sound Design</t>
   </si>
   <si>
     <t>Week 5</t>
@@ -178,7 +144,38 @@
     <t>July 17 - 22</t>
   </si>
   <si>
-    <t>Rough Launch Page</t>
+    <t>Come to Blossom St. on F, S</t>
+  </si>
+  <si>
+    <t>New Mechanics Coding</t>
+  </si>
+  <si>
+    <t>Implementing UI, Polish</t>
+  </si>
+  <si>
+    <t>Finish Level Design</t>
+  </si>
+  <si>
+    <t>Polish UI Assets</t>
+  </si>
+  <si>
+    <t>Marketing Research</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>July 24 - 29</t>
+  </si>
+  <si>
+    <t>28th</t>
+  </si>
+  <si>
+    <t>CONTENT
+COMPLETE + PLAYTEST</t>
+  </si>
+  <si>
+    <t>Rough Launch Page + FINAL PLAYTEST + LOCK BUILD</t>
   </si>
   <si>
     <t>LAUNCH</t>
@@ -187,7 +184,16 @@
     <t>Archive all Documents, Builds</t>
   </si>
   <si>
-    <t>Marketing Materials</t>
+    <t>QoL + Bugfixing</t>
+  </si>
+  <si>
+    <t>Final Level Design</t>
+  </si>
+  <si>
+    <t>Marketing Materials / Page Design</t>
+  </si>
+  <si>
+    <t>Post-Processing / Color Pass</t>
   </si>
   <si>
     <t>Itch.io Page Design</t>
@@ -203,10 +209,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mmmm d"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -235,8 +238,13 @@
       <name val="Open Sans"/>
     </font>
     <font/>
+    <font>
+      <b/>
+      <color rgb="FFEFEFEF"/>
+      <name val="Open Sans"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,8 +281,14 @@
         <bgColor rgb="FF6D9EEB"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6FA8DC"/>
+        <bgColor rgb="FF6FA8DC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -355,11 +369,19 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -413,7 +435,7 @@
     <xf borderId="7" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -425,22 +447,31 @@
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="8" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -476,8 +507,12 @@
       <c r="C1" s="3"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="2">
+        <v>23.0</v>
+      </c>
+      <c r="G1" s="2">
+        <v>24.0</v>
+      </c>
       <c r="H1" s="4"/>
     </row>
     <row r="2">
@@ -578,8 +613,12 @@
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="19"/>
+      <c r="F7" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.0</v>
+      </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8">
@@ -608,19 +647,15 @@
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="B9" s="19"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="D9" s="19"/>
       <c r="E9" s="9"/>
       <c r="F9" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H9" s="11"/>
     </row>
@@ -629,7 +664,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -643,39 +678,37 @@
         <v>15</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="17"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+        <v>27</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" ht="18.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
@@ -686,13 +719,13 @@
     </row>
     <row r="14">
       <c r="A14" s="4"/>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -707,81 +740,67 @@
       <c r="H14" s="6"/>
     </row>
     <row r="15">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="26"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="9"/>
+      <c r="B16" s="23" t="s">
+        <v>31</v>
+      </c>
       <c r="H16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="9"/>
+      <c r="B17" s="25" t="s">
+        <v>32</v>
+      </c>
       <c r="H17" s="9"/>
     </row>
     <row r="18">
       <c r="A18" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="16"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="G18" s="17"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" ht="18.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="F19" s="2">
+        <v>14.0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>15.0</v>
+      </c>
       <c r="H19" s="4"/>
     </row>
     <row r="20">
@@ -811,85 +830,75 @@
         <v>8</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>44</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="H21" s="10"/>
     </row>
     <row r="22">
       <c r="A22" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="13" t="s">
-        <v>46</v>
-      </c>
+      <c r="B22" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="11" t="s">
-        <v>47</v>
-      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="11"/>
     </row>
     <row r="23">
       <c r="A23" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="17"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="9"/>
     </row>
     <row r="24">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="B24" s="11"/>
       <c r="C24" s="10"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" ht="18.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="F25" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>22.0</v>
+      </c>
       <c r="H25" s="4"/>
     </row>
     <row r="26">
@@ -909,7 +918,7 @@
       <c r="F26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="28" t="s">
         <v>7</v>
       </c>
       <c r="H26" s="6"/>
@@ -918,102 +927,136 @@
       <c r="A27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="8" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H27" s="26"/>
+        <v>37</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="B28" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
       <c r="H28" s="9"/>
     </row>
     <row r="29">
       <c r="A29" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="B29" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="30"/>
       <c r="H29" s="9"/>
     </row>
     <row r="30">
       <c r="A30" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="15" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="2">
+        <v>26.0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>27.0</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
+      <c r="H33" s="31"/>
     </row>
     <row r="34">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
+      <c r="A34" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="17"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
@@ -1021,23 +1064,42 @@
       <c r="H34" s="9"/>
     </row>
     <row r="35">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
+      <c r="A35" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="17"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
     </row>
     <row r="36">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
+      <c r="A36" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>55</v>
+      </c>
       <c r="H36" s="9"/>
     </row>
     <row r="37">
@@ -10681,20 +10743,22 @@
       <c r="H1000" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B16:F16"/>
+  <mergeCells count="15">
     <mergeCell ref="B10:F10"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="E24:F24"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>